<commit_message>
edits to map and data
</commit_message>
<xml_diff>
--- a/archive/lit review africa health insurance coverage.xlsx
+++ b/archive/lit review africa health insurance coverage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uwnetid-my.sharepoint.com/personal/msahu_uw_edu/Documents/Documents/Research/IHME/FGH/Health insurance/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1053" documentId="8_{442C5DDD-C071-4E9F-A7F6-0E7C716F6C39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D182A016-EE45-410F-86C8-928C835FCE6D}"/>
+  <xr:revisionPtr revIDLastSave="180" documentId="8_{BCB08809-377C-40D1-8786-6BDE96F786D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{211D1B19-73A0-4718-9218-1D1883C0C1A0}"/>
   <bookViews>
-    <workbookView xWindow="8940" yWindow="4700" windowWidth="28800" windowHeight="15290" xr2:uid="{A077811C-20F4-4433-BB5B-D58A86C5C515}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12552" xr2:uid="{A077811C-20F4-4433-BB5B-D58A86C5C515}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="688" uniqueCount="241">
   <si>
     <t>Country</t>
   </si>
@@ -432,6 +432,9 @@
     <t>Barasa, 2021</t>
   </si>
   <si>
+    <t>National (public) health insurance?</t>
+  </si>
+  <si>
     <t>Ly, 2022; Barasa 2021</t>
   </si>
   <si>
@@ -708,14 +711,62 @@
     <t>Ly, 2022; Abdelaziz 2021</t>
   </si>
   <si>
-    <t xml:space="preserve">National (public) health insurance? </t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Yes, coverage &gt;40%</t>
+  </si>
+  <si>
+    <t>Yes, coverage &lt;40%</t>
+  </si>
+  <si>
+    <t>No, bill passed in 2023 but not yet implemented</t>
+  </si>
+  <si>
+    <t>Ly, 2022; https://www.pacificprime.com/country/africa/algeria-health-insurance-pacific-prime-international/</t>
+  </si>
+  <si>
+    <t>Yes, coverage unknown</t>
+  </si>
+  <si>
+    <t>No, planned but not implemented</t>
+  </si>
+  <si>
+    <t>https://equityhealthj.biomedcentral.com/articles/10.1186/s12939-023-01923-5</t>
+  </si>
+  <si>
+    <t>Kenya NHIF spending</t>
+  </si>
+  <si>
+    <t>Oyando</t>
+  </si>
+  <si>
+    <t>Barasa 2021; Oyanda 2023 (which cites DHS 2023)</t>
+  </si>
+  <si>
+    <t>National (public) health insurance? [old version]</t>
+  </si>
+  <si>
+    <t>Note: all of our estimates of coverage (&gt; or &lt; 40%) come from 2 papers (Ly 2021 and Barasa 2021) which rely on DHS data from 2010-2020, so may not be up to date ; need to make a note!</t>
+  </si>
+  <si>
+    <t>While this is not claims data in the traditional sense of the word where it is from the insurer's systems, the descriptions sounds like the database has the data on what they got from the insurer for treating the patient which to me captures items of interest. It will be interesting to see whether the cost reported in hospital differs from what insurers report in their systems. Do you have any idea here?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">While this article mentions claims processing, it reads more like a pilot and not real world claims processing so I would not count this article per se. </t>
+  </si>
+  <si>
+    <t>I think this is also claims data. However this is not granular patient related claims as we normally think of it but aggregated from the insurer perspective..so I think that is a caveat that we can also highlight in the commentary…the level of granularity even in what is available.</t>
+  </si>
+  <si>
+    <t>Angela's comments</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -739,8 +790,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -762,6 +828,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -794,7 +866,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
@@ -811,6 +883,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1130,28 +1208,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6FFE8C4-E496-408F-BFD9-4B000E87C643}">
-  <dimension ref="A1:J55"/>
+  <dimension ref="A1:K55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D1" sqref="D1"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="24.90625" customWidth="1"/>
-    <col min="2" max="2" width="6.08984375" customWidth="1"/>
-    <col min="3" max="3" width="5.36328125" customWidth="1"/>
-    <col min="4" max="4" width="15.6328125" customWidth="1"/>
-    <col min="5" max="5" width="12.26953125" customWidth="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1"/>
-    <col min="7" max="7" width="21.26953125" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="21.36328125" customWidth="1"/>
-    <col min="10" max="10" width="22.453125" customWidth="1"/>
+    <col min="1" max="1" width="21.62890625" customWidth="1"/>
+    <col min="2" max="2" width="6.1015625" customWidth="1"/>
+    <col min="3" max="3" width="5.3671875" customWidth="1"/>
+    <col min="4" max="4" width="21.89453125" customWidth="1"/>
+    <col min="5" max="5" width="26.734375" customWidth="1"/>
+    <col min="6" max="6" width="13.3671875" customWidth="1"/>
+    <col min="7" max="7" width="11.734375" customWidth="1"/>
+    <col min="8" max="8" width="21.3671875" customWidth="1"/>
+    <col min="9" max="9" width="14.5234375" customWidth="1"/>
+    <col min="10" max="10" width="21.3671875" customWidth="1"/>
+    <col min="11" max="11" width="18.62890625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="74" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="74.05" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1162,28 +1241,31 @@
         <v>54</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="G1" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="G1" s="5" t="s">
-        <v>213</v>
-      </c>
       <c r="H1" s="5" t="s">
-        <v>141</v>
+        <v>214</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>180</v>
+        <v>142</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K1" s="5" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="6" t="s">
         <v>55</v>
       </c>
@@ -1197,7 +1279,7 @@
         <v>52</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>53</v>
+        <v>225</v>
       </c>
       <c r="F2" s="6" t="s">
         <v>53</v>
@@ -1209,11 +1291,14 @@
         <v>53</v>
       </c>
       <c r="I2" s="6" t="s">
-        <v>123</v>
-      </c>
-      <c r="J2" s="6"/>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="K2" s="6"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="6" t="s">
         <v>56</v>
       </c>
@@ -1227,10 +1312,10 @@
         <v>53</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>53</v>
@@ -1239,11 +1324,14 @@
         <v>53</v>
       </c>
       <c r="I3" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="J3" s="6"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>136</v>
+      </c>
+      <c r="K3" s="6"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="6" t="s">
         <v>57</v>
       </c>
@@ -1257,23 +1345,26 @@
         <v>129</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="F4" s="6" t="s">
         <v>129</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="H4" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I4" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="J4" s="6"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="6" t="s">
         <v>58</v>
       </c>
@@ -1287,10 +1378,10 @@
         <v>53</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G5" s="6" t="s">
         <v>53</v>
@@ -1298,12 +1389,15 @@
       <c r="H5" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I5" s="7" t="s">
-        <v>139</v>
-      </c>
-      <c r="J5" s="6"/>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I5" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J5" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="K5" s="6"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="6" t="s">
         <v>59</v>
       </c>
@@ -1317,23 +1411,26 @@
         <v>129</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="F6" s="6" t="s">
         <v>129</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="H6" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J6" s="6"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K6" s="6"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="6" t="s">
         <v>60</v>
       </c>
@@ -1347,25 +1444,28 @@
         <v>52</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F7" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G7" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H7" s="6" t="s">
-        <v>53</v>
+      <c r="G7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H7" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="J7" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="6" t="s">
         <v>61</v>
       </c>
@@ -1379,10 +1479,10 @@
         <v>53</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G8" s="6" t="s">
         <v>53</v>
@@ -1391,11 +1491,14 @@
         <v>53</v>
       </c>
       <c r="I8" s="6" t="s">
-        <v>140</v>
-      </c>
-      <c r="J8" s="6"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>141</v>
+      </c>
+      <c r="K8" s="6"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="6" t="s">
         <v>62</v>
       </c>
@@ -1409,23 +1512,26 @@
         <v>129</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F9" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G9" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H9" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="J9" s="6"/>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="K9" s="6"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="6" t="s">
         <v>63</v>
       </c>
@@ -1439,7 +1545,7 @@
         <v>53</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>53</v>
+        <v>224</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>53</v>
@@ -1450,10 +1556,13 @@
       <c r="H10" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I10" s="6"/>
+      <c r="I10" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J10" s="6"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K10" s="6"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="6" t="s">
         <v>64</v>
       </c>
@@ -1467,23 +1576,26 @@
         <v>129</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="F11" s="6" t="s">
         <v>129</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="H11" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J11" s="6"/>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="6" t="s">
         <v>65</v>
       </c>
@@ -1497,25 +1609,28 @@
         <v>129</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H12" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J12" s="6"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K12" s="6"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="6" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>12</v>
@@ -1527,25 +1642,28 @@
         <v>129</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H13" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J13" s="6"/>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J13" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="6" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>13</v>
@@ -1557,25 +1675,28 @@
         <v>129</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F14" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G14" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H14" s="6" t="s">
-        <v>53</v>
+      <c r="G14" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H14" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="I14" s="6" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="J14" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="K14" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="6" t="s">
         <v>66</v>
       </c>
@@ -1589,23 +1710,26 @@
         <v>52</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F15" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H15" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I15" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J15" s="6"/>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J15" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K15" s="6"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="6" t="s">
         <v>67</v>
       </c>
@@ -1619,10 +1743,10 @@
         <v>52</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>52</v>
+        <v>229</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G16" s="6" t="s">
         <v>53</v>
@@ -1631,11 +1755,14 @@
         <v>53</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>143</v>
-      </c>
-      <c r="J16" s="6"/>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J16" s="6" t="s">
+        <v>144</v>
+      </c>
+      <c r="K16" s="6"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="6" t="s">
         <v>68</v>
       </c>
@@ -1649,10 +1776,10 @@
         <v>126</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>52</v>
+        <v>229</v>
       </c>
       <c r="F17" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>53</v>
@@ -1661,11 +1788,14 @@
         <v>53</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>142</v>
-      </c>
-      <c r="J17" s="6"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J17" s="6" t="s">
+        <v>143</v>
+      </c>
+      <c r="K17" s="6"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="6" t="s">
         <v>69</v>
       </c>
@@ -1679,10 +1809,10 @@
         <v>52</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>52</v>
+        <v>229</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G18" s="6" t="s">
         <v>53</v>
@@ -1690,12 +1820,15 @@
       <c r="H18" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I18" s="7" t="s">
-        <v>161</v>
-      </c>
-      <c r="J18" s="6"/>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I18" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="K18" s="6"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="6" t="s">
         <v>70</v>
       </c>
@@ -1706,13 +1839,13 @@
         <v>52</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>158</v>
+        <v>230</v>
       </c>
       <c r="F19" s="6" t="s">
-        <v>53</v>
+        <v>159</v>
       </c>
       <c r="G19" s="6" t="s">
         <v>53</v>
@@ -1721,13 +1854,16 @@
         <v>53</v>
       </c>
       <c r="I19" s="6" t="s">
-        <v>160</v>
-      </c>
-      <c r="J19" s="6"/>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J19" s="6" t="s">
+        <v>161</v>
+      </c>
+      <c r="K19" s="6"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="6" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>18</v>
@@ -1739,10 +1875,10 @@
         <v>53</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F20" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G20" s="6" t="s">
         <v>53</v>
@@ -1751,11 +1887,14 @@
         <v>53</v>
       </c>
       <c r="I20" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J20" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K20" s="6"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="6" t="s">
         <v>71</v>
       </c>
@@ -1769,25 +1908,28 @@
         <v>129</v>
       </c>
       <c r="E21" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F21" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>183</v>
-      </c>
-      <c r="H21" s="6" t="s">
-        <v>53</v>
+      <c r="G21" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="H21" s="8" t="s">
+        <v>184</v>
       </c>
       <c r="I21" s="6" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="J21" s="6" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+      <c r="K21" s="6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="6" t="s">
         <v>72</v>
       </c>
@@ -1801,10 +1943,10 @@
         <v>52</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>132</v>
+        <v>225</v>
       </c>
       <c r="F22" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="G22" s="6" t="s">
         <v>53</v>
@@ -1813,11 +1955,14 @@
         <v>53</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>162</v>
-      </c>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J22" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="K22" s="6"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="6" t="s">
         <v>73</v>
       </c>
@@ -1831,10 +1976,10 @@
         <v>52</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F23" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G23" s="6" t="s">
         <v>53</v>
@@ -1843,11 +1988,14 @@
         <v>53</v>
       </c>
       <c r="I23" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J23" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K23" s="6"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="6" t="s">
         <v>74</v>
       </c>
@@ -1861,25 +2009,28 @@
         <v>52</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>129</v>
+        <v>225</v>
       </c>
       <c r="F24" s="6" t="s">
         <v>129</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>52</v>
+        <v>129</v>
       </c>
       <c r="H24" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I24" s="6" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="J24" s="6" t="s">
-        <v>175</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+      <c r="K24" s="6" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="6" t="s">
         <v>75</v>
       </c>
@@ -1893,23 +2044,26 @@
         <v>129</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G25" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G25" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H25" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I25" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J25" s="6"/>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K25" s="6"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="6" t="s">
         <v>76</v>
       </c>
@@ -1923,23 +2077,26 @@
         <v>53</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F26" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H26" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I26" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="J26" s="6"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>157</v>
+      </c>
+      <c r="K26" s="6"/>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="6" t="s">
         <v>77</v>
       </c>
@@ -1952,24 +2109,27 @@
       <c r="D27" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E27" s="6" t="s">
-        <v>52</v>
+      <c r="E27" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="F27" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G27" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G27" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H27" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I27" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J27" s="6"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J27" s="6" t="s">
+        <v>234</v>
+      </c>
+      <c r="K27" s="6"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="6" t="s">
         <v>78</v>
       </c>
@@ -1983,23 +2143,26 @@
         <v>53</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F28" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G28" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H28" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="J28" s="6"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J28" s="6" t="s">
+        <v>160</v>
+      </c>
+      <c r="K28" s="6"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="6" t="s">
         <v>79</v>
       </c>
@@ -2013,23 +2176,26 @@
         <v>52</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H29" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J29" s="6"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K29" s="6"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="6" t="s">
         <v>80</v>
       </c>
@@ -2043,10 +2209,10 @@
         <v>53</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>132</v>
+        <v>224</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="G30" s="6" t="s">
         <v>53</v>
@@ -2055,11 +2221,14 @@
         <v>53</v>
       </c>
       <c r="I30" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="J30" s="6"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="K30" s="6"/>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="6" t="s">
         <v>81</v>
       </c>
@@ -2073,23 +2242,26 @@
         <v>52</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H31" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J31" s="6"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K31" s="6"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="6" t="s">
         <v>82</v>
       </c>
@@ -2103,10 +2275,10 @@
         <v>53</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F32" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G32" s="6" t="s">
         <v>53</v>
@@ -2115,11 +2287,14 @@
         <v>53</v>
       </c>
       <c r="I32" s="6" t="s">
-        <v>208</v>
-      </c>
-      <c r="J32" s="6"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>209</v>
+      </c>
+      <c r="K32" s="6"/>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="6" t="s">
         <v>83</v>
       </c>
@@ -2133,23 +2308,26 @@
         <v>52</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F33" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G33" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H33" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I33" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="J33" s="6"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J33" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K33" s="6"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="6" t="s">
         <v>84</v>
       </c>
@@ -2162,24 +2340,27 @@
       <c r="D34" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E34" s="6" t="s">
-        <v>132</v>
+      <c r="E34" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>52</v>
+        <v>133</v>
       </c>
       <c r="G34" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H34" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I34" s="7" t="s">
-        <v>165</v>
-      </c>
-      <c r="J34" s="6"/>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="I34" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J34" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="K34" s="6"/>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="6" t="s">
         <v>85</v>
       </c>
@@ -2193,10 +2374,10 @@
         <v>53</v>
       </c>
       <c r="E35" s="6" t="s">
-        <v>132</v>
+        <v>224</v>
       </c>
       <c r="F35" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="G35" s="6" t="s">
         <v>53</v>
@@ -2205,11 +2386,14 @@
         <v>53</v>
       </c>
       <c r="I35" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J35" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="J35" s="6"/>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K35" s="6"/>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="6" t="s">
         <v>86</v>
       </c>
@@ -2222,11 +2406,11 @@
       <c r="D36" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E36" s="6" t="s">
-        <v>132</v>
+      <c r="E36" s="10" t="s">
+        <v>225</v>
       </c>
       <c r="F36" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="G36" s="6" t="s">
         <v>53</v>
@@ -2235,11 +2419,14 @@
         <v>53</v>
       </c>
       <c r="I36" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J36" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="J36" s="6"/>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K36" s="6"/>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="6" t="s">
         <v>87</v>
       </c>
@@ -2253,10 +2440,10 @@
         <v>52</v>
       </c>
       <c r="E37" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G37" s="6" t="s">
         <v>53</v>
@@ -2265,11 +2452,14 @@
         <v>53</v>
       </c>
       <c r="I37" s="6" t="s">
-        <v>157</v>
-      </c>
-      <c r="J37" s="6"/>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J37" s="6" t="s">
+        <v>158</v>
+      </c>
+      <c r="K37" s="6"/>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="6" t="s">
         <v>88</v>
       </c>
@@ -2282,24 +2472,27 @@
       <c r="D38" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E38" s="6" t="s">
-        <v>52</v>
+      <c r="E38" s="10" t="s">
+        <v>226</v>
       </c>
       <c r="F38" s="6" t="s">
-        <v>132</v>
+        <v>52</v>
       </c>
       <c r="G38" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="H38" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I38" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J38" s="6"/>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J38" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K38" s="6"/>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="6" t="s">
         <v>89</v>
       </c>
@@ -2313,23 +2506,26 @@
         <v>52</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H39" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I39" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J39" s="6"/>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J39" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K39" s="6"/>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="6" t="s">
         <v>90</v>
       </c>
@@ -2343,23 +2539,26 @@
         <v>129</v>
       </c>
       <c r="E40" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F40" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G40" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H40" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I40" s="6" t="s">
-        <v>209</v>
-      </c>
-      <c r="J40" s="6"/>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="K40" s="6"/>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="6" t="s">
         <v>91</v>
       </c>
@@ -2373,25 +2572,28 @@
         <v>52</v>
       </c>
       <c r="E41" s="6" t="s">
+        <v>225</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="F41" s="6" t="s">
+      <c r="G41" s="6" t="s">
         <v>111</v>
       </c>
-      <c r="G41" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="H41" s="6" t="s">
-        <v>53</v>
+      <c r="H41" s="8" t="s">
+        <v>175</v>
       </c>
       <c r="I41" s="6" t="s">
-        <v>133</v>
+        <v>53</v>
       </c>
       <c r="J41" s="6" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.35">
+        <v>134</v>
+      </c>
+      <c r="K41" s="6" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="6" t="s">
         <v>92</v>
       </c>
@@ -2405,23 +2607,26 @@
         <v>129</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F42" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H42" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I42" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J42" s="6" t="s">
         <v>130</v>
       </c>
-      <c r="J42" s="6"/>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K42" s="6"/>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="6" t="s">
         <v>93</v>
       </c>
@@ -2432,26 +2637,29 @@
         <v>52</v>
       </c>
       <c r="D43" s="6" t="s">
-        <v>129</v>
+        <v>111</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>52</v>
+        <v>225</v>
       </c>
       <c r="F43" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G43" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H43" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I43" s="6" t="s">
-        <v>131</v>
-      </c>
-      <c r="J43" s="6"/>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J43" s="6" t="s">
+        <v>132</v>
+      </c>
+      <c r="K43" s="6"/>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="6" t="s">
         <v>94</v>
       </c>
@@ -2465,10 +2673,10 @@
         <v>53</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>132</v>
+        <v>224</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="G44" s="6" t="s">
         <v>53</v>
@@ -2476,10 +2684,13 @@
       <c r="H44" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I44" s="6"/>
+      <c r="I44" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J44" s="6"/>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K44" s="6"/>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="6" t="s">
         <v>95</v>
       </c>
@@ -2493,23 +2704,26 @@
         <v>129</v>
       </c>
       <c r="E45" s="6" t="s">
-        <v>129</v>
+        <v>226</v>
       </c>
       <c r="F45" s="6" t="s">
         <v>129</v>
       </c>
       <c r="G45" s="6" t="s">
-        <v>53</v>
+        <v>129</v>
       </c>
       <c r="H45" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I45" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J45" s="6"/>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J45" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K45" s="6"/>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="6" t="s">
         <v>96</v>
       </c>
@@ -2523,10 +2737,10 @@
         <v>53</v>
       </c>
       <c r="E46" s="6" t="s">
-        <v>52</v>
+        <v>224</v>
       </c>
       <c r="F46" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G46" s="6" t="s">
         <v>53</v>
@@ -2535,11 +2749,14 @@
         <v>53</v>
       </c>
       <c r="I46" s="6" t="s">
-        <v>167</v>
-      </c>
-      <c r="J46" s="6"/>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J46" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="K46" s="6"/>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="6" t="s">
         <v>97</v>
       </c>
@@ -2550,26 +2767,29 @@
         <v>52</v>
       </c>
       <c r="D47" s="6" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="E47" s="6" t="s">
-        <v>52</v>
+        <v>227</v>
       </c>
       <c r="F47" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>218</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
+      </c>
+      <c r="G47" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="H47" s="8" t="s">
+        <v>219</v>
       </c>
       <c r="I47" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="J47" s="6"/>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="K47" s="6"/>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="6" t="s">
         <v>98</v>
       </c>
@@ -2583,7 +2803,7 @@
         <v>53</v>
       </c>
       <c r="E48" s="6" t="s">
-        <v>53</v>
+        <v>224</v>
       </c>
       <c r="F48" s="6" t="s">
         <v>53</v>
@@ -2594,10 +2814,13 @@
       <c r="H48" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="I48" s="6"/>
+      <c r="I48" s="6" t="s">
+        <v>53</v>
+      </c>
       <c r="J48" s="6"/>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K48" s="6"/>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="6" t="s">
         <v>99</v>
       </c>
@@ -2610,11 +2833,11 @@
       <c r="D49" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E49" s="6" t="s">
-        <v>52</v>
+      <c r="E49" s="10" t="s">
+        <v>225</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="G49" s="6" t="s">
         <v>53</v>
@@ -2623,11 +2846,14 @@
         <v>53</v>
       </c>
       <c r="I49" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="J49" s="6" t="s">
         <v>123</v>
       </c>
-      <c r="J49" s="6"/>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
+      <c r="K49" s="6"/>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="6" t="s">
         <v>100</v>
       </c>
@@ -2641,7 +2867,7 @@
         <v>52</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F50" s="6" t="s">
         <v>52</v>
@@ -2650,16 +2876,19 @@
         <v>52</v>
       </c>
       <c r="H50" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I50" s="6" t="s">
-        <v>131</v>
+        <v>53</v>
       </c>
       <c r="J50" s="6" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.35">
+        <v>132</v>
+      </c>
+      <c r="K50" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="6" t="s">
         <v>101</v>
       </c>
@@ -2673,23 +2902,26 @@
         <v>52</v>
       </c>
       <c r="E51" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F51" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G51" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G51" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H51" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I51" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="J51" s="6"/>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J51" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="K51" s="6"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="6" t="s">
         <v>102</v>
       </c>
@@ -2702,11 +2934,11 @@
       <c r="D52" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="E52" s="6" t="s">
-        <v>132</v>
+      <c r="E52" s="10" t="s">
+        <v>225</v>
       </c>
       <c r="F52" s="6" t="s">
-        <v>53</v>
+        <v>133</v>
       </c>
       <c r="G52" s="6" t="s">
         <v>53</v>
@@ -2715,11 +2947,14 @@
         <v>53</v>
       </c>
       <c r="I52" s="6" t="s">
-        <v>222</v>
-      </c>
-      <c r="J52" s="6"/>
-    </row>
-    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J52" s="6" t="s">
+        <v>223</v>
+      </c>
+      <c r="K52" s="6"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="6" t="s">
         <v>103</v>
       </c>
@@ -2733,23 +2968,26 @@
         <v>53</v>
       </c>
       <c r="E53" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F53" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G53" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H53" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I53" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="J53" s="6"/>
-    </row>
-    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J53" s="6" t="s">
+        <v>139</v>
+      </c>
+      <c r="K53" s="6"/>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="6" t="s">
         <v>104</v>
       </c>
@@ -2763,23 +3001,26 @@
         <v>129</v>
       </c>
       <c r="E54" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F54" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="G54" s="6" t="s">
         <v>129</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>53</v>
-      </c>
       <c r="H54" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I54" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J54" s="6"/>
-    </row>
-    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
+        <v>53</v>
+      </c>
+      <c r="J54" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K54" s="6"/>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="6" t="s">
         <v>105</v>
       </c>
@@ -2793,27 +3034,30 @@
         <v>129</v>
       </c>
       <c r="E55" s="6" t="s">
-        <v>52</v>
+        <v>226</v>
       </c>
       <c r="F55" s="6" t="s">
         <v>52</v>
       </c>
       <c r="G55" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="H55" s="6" t="s">
         <v>53</v>
       </c>
       <c r="I55" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="J55" s="6"/>
+        <v>53</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="K55" s="6"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="I18" r:id="rId1" display="https://www.allianzcare.com/en/about-us/news/2016/04/comprehensive-health-insurance-plans-for-equatorial-guinea.html" xr:uid="{9392446C-3ABA-4BFC-BF36-D7CF64C38293}"/>
-    <hyperlink ref="I34" r:id="rId2" display="https://openimis.org/mauritania-health-insurance" xr:uid="{87DBE969-1C17-48E2-AE56-962B30EA18C1}"/>
-    <hyperlink ref="I5" r:id="rId3" xr:uid="{74CD4B01-5599-415F-BCA4-1A8FE2CBCDC9}"/>
+    <hyperlink ref="J18" r:id="rId1" display="https://www.allianzcare.com/en/about-us/news/2016/04/comprehensive-health-insurance-plans-for-equatorial-guinea.html" xr:uid="{9392446C-3ABA-4BFC-BF36-D7CF64C38293}"/>
+    <hyperlink ref="J34" r:id="rId2" display="https://openimis.org/mauritania-health-insurance" xr:uid="{87DBE969-1C17-48E2-AE56-962B30EA18C1}"/>
+    <hyperlink ref="J5" r:id="rId3" xr:uid="{74CD4B01-5599-415F-BCA4-1A8FE2CBCDC9}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -2822,24 +3066,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42977400-B5F8-4F2A-A40E-0559A5BCB22D}">
-  <dimension ref="A1:G23"/>
+  <dimension ref="A1:H27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="14.6328125" customWidth="1"/>
-    <col min="2" max="2" width="14.26953125" customWidth="1"/>
-    <col min="3" max="3" width="5.90625" customWidth="1"/>
-    <col min="4" max="4" width="7.7265625" customWidth="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1"/>
-    <col min="6" max="6" width="37.1796875" customWidth="1"/>
-    <col min="7" max="7" width="33.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.62890625" customWidth="1"/>
+    <col min="2" max="2" width="14.26171875" customWidth="1"/>
+    <col min="3" max="3" width="5.89453125" customWidth="1"/>
+    <col min="4" max="4" width="7.734375" customWidth="1"/>
+    <col min="5" max="5" width="10.15625" customWidth="1"/>
+    <col min="6" max="6" width="37.15625" customWidth="1"/>
+    <col min="7" max="7" width="33.7890625" customWidth="1"/>
+    <col min="8" max="8" width="14.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="3" t="s">
         <v>115</v>
       </c>
@@ -2856,15 +3101,18 @@
         <v>117</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="13" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="B2" t="s">
         <v>120</v>
@@ -2882,9 +3130,9 @@
         <v>114</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="B3" t="s">
         <v>120</v>
@@ -2898,13 +3146,13 @@
       <c r="E3" t="s">
         <v>53</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C4">
         <v>2023</v>
@@ -2913,9 +3161,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C5">
         <v>2021</v>
@@ -2927,9 +3175,9 @@
         <v>118</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B6" t="s">
         <v>91</v>
@@ -2947,7 +3195,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>124</v>
       </c>
@@ -2967,9 +3215,9 @@
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="B8" t="s">
         <v>120</v>
@@ -2987,9 +3235,9 @@
         <v>127</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B9" t="s">
         <v>100</v>
@@ -3004,9 +3252,9 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="B10" t="s">
         <v>100</v>
@@ -3021,12 +3269,12 @@
         <v>111</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B11" t="s">
         <v>76</v>
@@ -3038,15 +3286,15 @@
         <v>53</v>
       </c>
       <c r="E11" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="G11" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B12" t="s">
         <v>57</v>
@@ -3061,18 +3309,18 @@
         <v>53</v>
       </c>
       <c r="F12" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G12" t="s">
-        <v>170</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="1" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="C13" s="1">
         <v>2019</v>
@@ -3081,18 +3329,21 @@
         <v>53</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="F13" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>194</v>
-      </c>
       <c r="G13" s="9" t="s">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+        <v>174</v>
+      </c>
+      <c r="H13" s="11" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="1" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>74</v>
@@ -3107,15 +3358,18 @@
         <v>52</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+        <v>178</v>
+      </c>
+      <c r="H14" s="11" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B15" t="s">
         <v>99</v>
@@ -3124,21 +3378,22 @@
         <v>2022</v>
       </c>
       <c r="D15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="E15" t="s">
         <v>53</v>
       </c>
       <c r="F15" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="G15" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+        <v>180</v>
+      </c>
+      <c r="H15" s="12"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="1" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>71</v>
@@ -3153,18 +3408,21 @@
         <v>52</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+        <v>187</v>
+      </c>
+      <c r="H16" s="11" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B17" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C17">
         <v>2021</v>
@@ -3176,15 +3434,15 @@
         <v>53</v>
       </c>
       <c r="F17" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="G17" t="s">
-        <v>190</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B18" t="s">
         <v>98</v>
@@ -3196,18 +3454,18 @@
         <v>53</v>
       </c>
       <c r="E18" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F18" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G18" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B19" t="s">
         <v>98</v>
@@ -3222,15 +3480,15 @@
         <v>53</v>
       </c>
       <c r="F19" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G19" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B20" t="s">
         <v>82</v>
@@ -3245,15 +3503,15 @@
         <v>53</v>
       </c>
       <c r="F20" t="s">
+        <v>208</v>
+      </c>
+      <c r="G20" t="s">
         <v>207</v>
       </c>
-      <c r="G20" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
         <v>90</v>
@@ -3268,15 +3526,15 @@
         <v>53</v>
       </c>
       <c r="F21" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="G21" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B22" t="s">
         <v>101</v>
@@ -3291,15 +3549,15 @@
         <v>53</v>
       </c>
       <c r="F22" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G22" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B23" t="s">
         <v>102</v>
@@ -3314,10 +3572,38 @@
         <v>53</v>
       </c>
       <c r="F23" t="s">
+        <v>222</v>
+      </c>
+      <c r="G23" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="G23" t="s">
-        <v>220</v>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" t="s">
+        <v>233</v>
+      </c>
+      <c r="B24" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24">
+        <v>2023</v>
+      </c>
+      <c r="D24" t="s">
+        <v>53</v>
+      </c>
+      <c r="E24" t="s">
+        <v>53</v>
+      </c>
+      <c r="F24" t="s">
+        <v>232</v>
+      </c>
+      <c r="G24" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" t="s">
+        <v>236</v>
       </c>
     </row>
   </sheetData>
@@ -3325,9 +3611,11 @@
     <hyperlink ref="G10" r:id="rId1" xr:uid="{F8C20228-D649-4E99-BED7-2310CE384CD7}"/>
     <hyperlink ref="G8" r:id="rId2" xr:uid="{3E96E692-80AC-4963-8314-22E911080757}"/>
     <hyperlink ref="G13" r:id="rId3" xr:uid="{940E0A87-10C2-4C02-9F4F-37FD96FB6151}"/>
+    <hyperlink ref="G3" r:id="rId4" xr:uid="{76E82697-307E-47BE-9CA2-60E84E2F28DE}"/>
+    <hyperlink ref="G23" r:id="rId5" xr:uid="{A84051E2-7C96-4882-BE1B-66B34A8024BA}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>